<commit_message>
Updating daily files July 27
</commit_message>
<xml_diff>
--- a/assets/Top Prop Lines.xlsx
+++ b/assets/Top Prop Lines.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="114">
   <si>
     <t>fg_name</t>
   </si>
@@ -202,133 +202,163 @@
     <t>Seiya Suzuki</t>
   </si>
   <si>
+    <t>Manny Machado</t>
+  </si>
+  <si>
     <t>Luis Arraez</t>
   </si>
   <si>
-    <t>Royce Lewis</t>
-  </si>
-  <si>
-    <t>Jarren Duran</t>
-  </si>
-  <si>
-    <t>Adam Frazier</t>
-  </si>
-  <si>
-    <t>Jorge Soler</t>
+    <t>Jackson Merrill</t>
+  </si>
+  <si>
+    <t>Yandy Diaz</t>
+  </si>
+  <si>
+    <t>George Springer</t>
+  </si>
+  <si>
+    <t>Juan Soto</t>
   </si>
   <si>
     <t>Steven Kwan</t>
   </si>
   <si>
+    <t>Masyn Winn</t>
+  </si>
+  <si>
     <t>Chicago Cubs</t>
   </si>
   <si>
     <t>San Diego Padres</t>
   </si>
   <si>
-    <t>Minnesota Twins</t>
+    <t>Tampa Bay Rays</t>
+  </si>
+  <si>
+    <t>Toronto Blue Jays</t>
+  </si>
+  <si>
+    <t>New York Yankees</t>
+  </si>
+  <si>
+    <t>Cleveland Indians</t>
+  </si>
+  <si>
+    <t>St. Louis Cardinals</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>vs R</t>
+  </si>
+  <si>
+    <t>vs L</t>
+  </si>
+  <si>
+    <t>Seth Lugo</t>
+  </si>
+  <si>
+    <t>Dean Kremer</t>
+  </si>
+  <si>
+    <t>Andrew Abbott</t>
+  </si>
+  <si>
+    <t>Michael Lorenzen</t>
+  </si>
+  <si>
+    <t>Kutter Crawford</t>
+  </si>
+  <si>
+    <t>Tyler Phillips</t>
+  </si>
+  <si>
+    <t>Jake Irvin</t>
+  </si>
+  <si>
+    <t>Kansas City Royals</t>
+  </si>
+  <si>
+    <t>Baltimore Orioles</t>
+  </si>
+  <si>
+    <t>Cincinnati Reds</t>
+  </si>
+  <si>
+    <t>Texas Rangers</t>
   </si>
   <si>
     <t>Boston Red Sox</t>
   </si>
   <si>
-    <t>Kansas City Royals</t>
+    <t>Philadelphia Phillies</t>
+  </si>
+  <si>
+    <t>Washington Nationals</t>
+  </si>
+  <si>
+    <t>RHP</t>
+  </si>
+  <si>
+    <t>LHP</t>
+  </si>
+  <si>
+    <t>hits</t>
+  </si>
+  <si>
+    <t>draftkings</t>
+  </si>
+  <si>
+    <t>2024-07-27T23:11:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-27T20:06:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-27T20:11:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-27T19:08:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-27T23:16:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-27T22:06:00Z</t>
+  </si>
+  <si>
+    <t>Cleveland Guardians</t>
+  </si>
+  <si>
+    <t>Tyler Fitzgerald</t>
+  </si>
+  <si>
+    <t>Yordan Alvarez</t>
   </si>
   <si>
     <t>San Francisco Giants</t>
   </si>
   <si>
-    <t>Cleveland Indians</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>vs R</t>
-  </si>
-  <si>
-    <t>vs L</t>
-  </si>
-  <si>
-    <t>Brady Singer</t>
-  </si>
-  <si>
-    <t>G. Rodriguez</t>
-  </si>
-  <si>
-    <t>Keider Montero</t>
-  </si>
-  <si>
-    <t>Nestor Cortes</t>
-  </si>
-  <si>
-    <t>Kyle Hendricks</t>
-  </si>
-  <si>
-    <t>Kyle Freeland</t>
-  </si>
-  <si>
-    <t>C. Sanchez</t>
-  </si>
-  <si>
-    <t>Baltimore Orioles</t>
-  </si>
-  <si>
-    <t>Detroit Tigers</t>
-  </si>
-  <si>
-    <t>New York Yankees</t>
+    <t>Houston Astros</t>
+  </si>
+  <si>
+    <t>Tanner Gordon</t>
+  </si>
+  <si>
+    <t>Justin Wrobleski</t>
   </si>
   <si>
     <t>Colorado Rockies</t>
   </si>
   <si>
-    <t>Philadelphia Phillies</t>
-  </si>
-  <si>
-    <t>RHP</t>
-  </si>
-  <si>
-    <t>LHP</t>
-  </si>
-  <si>
-    <t>Grayson Rodriguez</t>
-  </si>
-  <si>
-    <t>Cristopher Sánchez</t>
-  </si>
-  <si>
-    <t>hits</t>
-  </si>
-  <si>
-    <t>draftkings</t>
-  </si>
-  <si>
-    <t>2024-07-27T00:11:00Z</t>
-  </si>
-  <si>
-    <t>2024-07-26T23:06:00Z</t>
-  </si>
-  <si>
-    <t>2024-07-26T22:41:00Z</t>
-  </si>
-  <si>
-    <t>2024-07-26T23:11:00Z</t>
-  </si>
-  <si>
-    <t>2024-07-27T02:16:00Z</t>
-  </si>
-  <si>
-    <t>Cleveland Guardians</t>
-  </si>
-  <si>
-    <t>David Villar</t>
-  </si>
-  <si>
-    <t>Tyler Fitzgerald</t>
+    <t>Los Angeles Dodgers</t>
+  </si>
+  <si>
+    <t>2024-07-27T23:05:00Z</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1094,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE9"/>
+  <dimension ref="A1:BE11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1248,7 +1278,7 @@
         <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>59</v>
@@ -1257,16 +1287,16 @@
         <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -1278,97 +1308,97 @@
         <v>2</v>
       </c>
       <c r="L2">
-        <v>0.253</v>
+        <v>0.25</v>
       </c>
       <c r="M2">
-        <v>0.307</v>
+        <v>0.304</v>
       </c>
       <c r="N2">
-        <v>0.106</v>
+        <v>0.105</v>
       </c>
       <c r="O2">
-        <v>0.329</v>
+        <v>0.326</v>
       </c>
       <c r="P2">
-        <v>0.358</v>
+        <v>0.355</v>
       </c>
       <c r="Q2">
-        <v>0.6879999999999999</v>
+        <v>0.681</v>
       </c>
       <c r="R2">
-        <v>10</v>
+        <v>10.2</v>
       </c>
       <c r="S2">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
       <c r="T2">
-        <v>47.1</v>
+        <v>46.8</v>
       </c>
       <c r="U2">
-        <v>30.8</v>
+        <v>31.3</v>
       </c>
       <c r="V2">
-        <v>19</v>
+        <v>18.9</v>
       </c>
       <c r="W2" t="s">
+        <v>80</v>
+      </c>
+      <c r="X2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" t="s">
         <v>78</v>
       </c>
-      <c r="X2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>76</v>
-      </c>
       <c r="AC2">
-        <v>210</v>
+        <v>256</v>
       </c>
       <c r="AD2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AE2">
-        <v>0.174</v>
+        <v>0.205</v>
       </c>
       <c r="AF2">
-        <v>0.219</v>
+        <v>0.256</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="AH2">
-        <v>0.082</v>
+        <v>0.138</v>
       </c>
       <c r="AI2">
-        <v>0.256</v>
+        <v>0.343</v>
       </c>
       <c r="AJ2">
-        <v>25.2</v>
+        <v>21.1</v>
       </c>
       <c r="AK2">
-        <v>4.8</v>
+        <v>3.9</v>
       </c>
       <c r="AL2">
-        <v>2.47</v>
+        <v>3.47</v>
       </c>
       <c r="AM2">
-        <v>47.5</v>
+        <v>40.6</v>
       </c>
       <c r="AN2">
-        <v>32.6</v>
+        <v>42.8</v>
       </c>
       <c r="AO2">
-        <v>4.3</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="AP2">
-        <v>25.2</v>
+        <v>32.3</v>
       </c>
       <c r="AQ2">
         <v>0</v>
@@ -1392,28 +1422,28 @@
         <v>59</v>
       </c>
       <c r="AX2">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="AY2">
         <v>1.5</v>
       </c>
       <c r="AZ2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BC2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="BD2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="BE2">
-        <v>-220</v>
+        <v>-195</v>
       </c>
     </row>
     <row r="3" spans="1:57">
@@ -1421,7 +1451,7 @@
         <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -1430,16 +1460,16 @@
         <v>60</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="I3">
         <v>11</v>
@@ -1451,97 +1481,97 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <v>0.265</v>
+        <v>0.27</v>
       </c>
       <c r="M3">
+        <v>0.349</v>
+      </c>
+      <c r="N3">
+        <v>0.211</v>
+      </c>
+      <c r="O3">
+        <v>0.331</v>
+      </c>
+      <c r="P3">
+        <v>0.481</v>
+      </c>
+      <c r="Q3">
+        <v>0.8120000000000001</v>
+      </c>
+      <c r="R3">
+        <v>30.4</v>
+      </c>
+      <c r="S3">
+        <v>7.2</v>
+      </c>
+      <c r="T3">
+        <v>35.6</v>
+      </c>
+      <c r="U3">
+        <v>46.3</v>
+      </c>
+      <c r="V3">
+        <v>37.5</v>
+      </c>
+      <c r="W3" t="s">
+        <v>80</v>
+      </c>
+      <c r="X3" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC3">
+        <v>256</v>
+      </c>
+      <c r="AD3">
+        <v>7</v>
+      </c>
+      <c r="AE3">
+        <v>0.205</v>
+      </c>
+      <c r="AF3">
+        <v>0.256</v>
+      </c>
+      <c r="AG3">
+        <v>2.7</v>
+      </c>
+      <c r="AH3">
+        <v>0.138</v>
+      </c>
+      <c r="AI3">
         <v>0.343</v>
       </c>
-      <c r="N3">
-        <v>0.209</v>
-      </c>
-      <c r="O3">
-        <v>0.324</v>
-      </c>
-      <c r="P3">
-        <v>0.474</v>
-      </c>
-      <c r="Q3">
-        <v>0.799</v>
-      </c>
-      <c r="R3">
-        <v>30.9</v>
-      </c>
-      <c r="S3">
-        <v>6.9</v>
-      </c>
-      <c r="T3">
-        <v>35</v>
-      </c>
-      <c r="U3">
-        <v>46.5</v>
-      </c>
-      <c r="V3">
-        <v>37.6</v>
-      </c>
-      <c r="W3" t="s">
-        <v>78</v>
-      </c>
-      <c r="X3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC3">
-        <v>210</v>
-      </c>
-      <c r="AD3">
-        <v>2</v>
-      </c>
-      <c r="AE3">
-        <v>0.174</v>
-      </c>
-      <c r="AF3">
-        <v>0.219</v>
-      </c>
-      <c r="AG3">
-        <v>1</v>
-      </c>
-      <c r="AH3">
-        <v>0.082</v>
-      </c>
-      <c r="AI3">
-        <v>0.256</v>
-      </c>
       <c r="AJ3">
-        <v>25.2</v>
+        <v>21.1</v>
       </c>
       <c r="AK3">
-        <v>4.8</v>
+        <v>3.9</v>
       </c>
       <c r="AL3">
-        <v>2.47</v>
+        <v>3.47</v>
       </c>
       <c r="AM3">
-        <v>47.5</v>
+        <v>40.6</v>
       </c>
       <c r="AN3">
-        <v>32.6</v>
+        <v>42.8</v>
       </c>
       <c r="AO3">
-        <v>4.3</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="AP3">
-        <v>25.2</v>
+        <v>32.3</v>
       </c>
       <c r="AQ3">
         <v>1</v>
@@ -1565,28 +1595,28 @@
         <v>60</v>
       </c>
       <c r="AX3">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="AY3">
         <v>1.5</v>
       </c>
       <c r="AZ3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BC3" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="BD3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="BE3">
-        <v>-280</v>
+        <v>-240</v>
       </c>
     </row>
     <row r="4" spans="1:57">
@@ -1594,7 +1624,7 @@
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>61</v>
@@ -1603,118 +1633,118 @@
         <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.323</v>
+        <v>0.268</v>
       </c>
       <c r="M4">
-        <v>0.331</v>
+        <v>0.312</v>
       </c>
       <c r="N4">
-        <v>0.08500000000000001</v>
+        <v>0.146</v>
       </c>
       <c r="O4">
-        <v>0.352</v>
+        <v>0.309</v>
       </c>
       <c r="P4">
-        <v>0.408</v>
+        <v>0.414</v>
       </c>
       <c r="Q4">
-        <v>0.759</v>
+        <v>0.723</v>
       </c>
       <c r="R4">
-        <v>2.6</v>
+        <v>20.8</v>
       </c>
       <c r="S4">
-        <v>4</v>
+        <v>5.4</v>
       </c>
       <c r="T4">
-        <v>37</v>
+        <v>46.8</v>
       </c>
       <c r="U4">
-        <v>30.7</v>
+        <v>33.5</v>
       </c>
       <c r="V4">
-        <v>24.8</v>
+        <v>35.6</v>
       </c>
       <c r="W4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="X4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="Y4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Z4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="AA4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AB4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AC4">
-        <v>217</v>
+        <v>144</v>
       </c>
       <c r="AD4">
         <v>4</v>
       </c>
       <c r="AE4">
-        <v>0.202</v>
+        <v>0.209</v>
       </c>
       <c r="AF4">
         <v>0.264</v>
       </c>
       <c r="AG4">
-        <v>1.8</v>
+        <v>2.8</v>
       </c>
       <c r="AH4">
-        <v>0.116</v>
+        <v>0.124</v>
       </c>
       <c r="AI4">
-        <v>0.318</v>
+        <v>0.333</v>
       </c>
       <c r="AJ4">
-        <v>29</v>
+        <v>23.6</v>
       </c>
       <c r="AK4">
-        <v>8.300000000000001</v>
+        <v>6.3</v>
       </c>
       <c r="AL4">
-        <v>2.83</v>
+        <v>3.64</v>
       </c>
       <c r="AM4">
-        <v>43</v>
+        <v>41.8</v>
       </c>
       <c r="AN4">
-        <v>37.8</v>
+        <v>40.8</v>
       </c>
       <c r="AO4">
-        <v>7.8</v>
+        <v>10</v>
       </c>
       <c r="AP4">
-        <v>31.9</v>
+        <v>29.3</v>
       </c>
       <c r="AQ4">
         <v>0</v>
@@ -1723,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="AS4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT4">
         <v>0</v>
@@ -1732,34 +1762,34 @@
         <v>0</v>
       </c>
       <c r="AV4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW4" t="s">
         <v>61</v>
       </c>
       <c r="AX4">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="AY4">
         <v>1.5</v>
       </c>
       <c r="AZ4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="BC4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="BD4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="BE4">
-        <v>-205</v>
+        <v>-260</v>
       </c>
     </row>
     <row r="5" spans="1:57">
@@ -1767,7 +1797,7 @@
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>62</v>
@@ -1776,121 +1806,121 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>264</v>
+      </c>
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="H5">
-        <v>65</v>
-      </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
       <c r="J5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>0.246</v>
+        <v>0.322</v>
       </c>
       <c r="M5">
-        <v>0.401</v>
+        <v>0.33</v>
       </c>
       <c r="N5">
-        <v>0.415</v>
+        <v>0.083</v>
       </c>
       <c r="O5">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="P5">
-        <v>0.662</v>
+        <v>0.405</v>
       </c>
       <c r="Q5">
-        <v>0.962</v>
+        <v>0.755</v>
       </c>
       <c r="R5">
-        <v>21.4</v>
+        <v>2.5</v>
       </c>
       <c r="S5">
-        <v>7.1</v>
+        <v>4</v>
       </c>
       <c r="T5">
-        <v>38</v>
+        <v>37.6</v>
       </c>
       <c r="U5">
-        <v>42</v>
+        <v>30.6</v>
       </c>
       <c r="V5">
-        <v>40</v>
+        <v>25.6</v>
       </c>
       <c r="W5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="X5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Y5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Z5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AA5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AC5">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="AD5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AE5">
-        <v>0.281</v>
+        <v>0.221</v>
       </c>
       <c r="AF5">
-        <v>0.413</v>
+        <v>0.344</v>
       </c>
       <c r="AG5">
-        <v>7.9</v>
+        <v>6.6</v>
       </c>
       <c r="AH5">
-        <v>0.351</v>
+        <v>0.26</v>
       </c>
       <c r="AI5">
-        <v>0.632</v>
+        <v>0.481</v>
       </c>
       <c r="AJ5">
-        <v>17.5</v>
+        <v>21.2</v>
       </c>
       <c r="AK5">
-        <v>9.5</v>
+        <v>12.6</v>
       </c>
       <c r="AL5">
-        <v>7.5</v>
+        <v>6.69</v>
       </c>
       <c r="AM5">
-        <v>23.9</v>
+        <v>39.4</v>
       </c>
       <c r="AN5">
-        <v>52.2</v>
+        <v>45.5</v>
       </c>
       <c r="AO5">
-        <v>20.8</v>
+        <v>22.2</v>
       </c>
       <c r="AP5">
-        <v>47.8</v>
+        <v>34</v>
       </c>
       <c r="AQ5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR5">
         <v>0</v>
@@ -1899,40 +1929,40 @@
         <v>0</v>
       </c>
       <c r="AT5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW5" t="s">
         <v>62</v>
       </c>
       <c r="AX5">
-        <v>195</v>
+        <v>140</v>
       </c>
       <c r="AY5">
         <v>1.5</v>
       </c>
       <c r="AZ5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="BC5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="BD5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BE5">
-        <v>-275</v>
+        <v>-190</v>
       </c>
     </row>
     <row r="6" spans="1:57">
@@ -1949,67 +1979,67 @@
         <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H6">
-        <v>133</v>
+        <v>252</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <v>2</v>
       </c>
       <c r="L6">
-        <v>0.271</v>
+        <v>0.317</v>
       </c>
       <c r="M6">
-        <v>0.317</v>
+        <v>0.36</v>
       </c>
       <c r="N6">
-        <v>0.09</v>
+        <v>0.167</v>
       </c>
       <c r="O6">
-        <v>0.347</v>
+        <v>0.351</v>
       </c>
       <c r="P6">
-        <v>0.361</v>
+        <v>0.484</v>
       </c>
       <c r="Q6">
-        <v>0.708</v>
+        <v>0.835</v>
       </c>
       <c r="R6">
-        <v>24.5</v>
+        <v>20.2</v>
       </c>
       <c r="S6">
-        <v>8.6</v>
+        <v>4.5</v>
       </c>
       <c r="T6">
-        <v>61.3</v>
+        <v>36</v>
       </c>
       <c r="U6">
-        <v>22.6</v>
+        <v>36.5</v>
       </c>
       <c r="V6">
-        <v>29.6</v>
+        <v>33.5</v>
       </c>
       <c r="W6" t="s">
         <v>81</v>
       </c>
       <c r="X6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Y6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Z6" t="s">
         <v>70</v>
@@ -2018,64 +2048,64 @@
         <v>81</v>
       </c>
       <c r="AB6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AC6">
-        <v>88</v>
+        <v>151</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AE6">
-        <v>0.217</v>
+        <v>0.221</v>
       </c>
       <c r="AF6">
-        <v>0.242</v>
+        <v>0.344</v>
       </c>
       <c r="AG6">
-        <v>1.1</v>
+        <v>6.6</v>
       </c>
       <c r="AH6">
-        <v>0.08400000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="AI6">
-        <v>0.301</v>
+        <v>0.481</v>
       </c>
       <c r="AJ6">
-        <v>27.3</v>
+        <v>21.2</v>
       </c>
       <c r="AK6">
-        <v>4.5</v>
+        <v>12.6</v>
       </c>
       <c r="AL6">
-        <v>2.1</v>
+        <v>6.69</v>
       </c>
       <c r="AM6">
-        <v>23.3</v>
+        <v>39.4</v>
       </c>
       <c r="AN6">
-        <v>50</v>
+        <v>45.5</v>
       </c>
       <c r="AO6">
-        <v>3.3</v>
+        <v>22.2</v>
       </c>
       <c r="AP6">
-        <v>26.7</v>
+        <v>34</v>
       </c>
       <c r="AQ6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT6">
         <v>0</v>
       </c>
       <c r="AU6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV6">
         <v>0</v>
@@ -2084,28 +2114,28 @@
         <v>63</v>
       </c>
       <c r="AX6">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="AY6">
         <v>1.5</v>
       </c>
       <c r="AZ6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB6" t="s">
         <v>99</v>
       </c>
       <c r="BC6" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD6" t="s">
         <v>70</v>
       </c>
-      <c r="BD6" t="s">
-        <v>87</v>
-      </c>
       <c r="BE6">
-        <v>-240</v>
+        <v>-265</v>
       </c>
     </row>
     <row r="7" spans="1:57">
@@ -2122,67 +2152,67 @@
         <v>64</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>162</v>
+        <v>94</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.191</v>
+        <v>0.33</v>
       </c>
       <c r="M7">
-        <v>0.258</v>
+        <v>0.365</v>
       </c>
       <c r="N7">
-        <v>0.099</v>
+        <v>0.16</v>
       </c>
       <c r="O7">
-        <v>0.276</v>
+        <v>0.363</v>
       </c>
       <c r="P7">
-        <v>0.29</v>
+        <v>0.489</v>
       </c>
       <c r="Q7">
-        <v>0.5659999999999999</v>
+        <v>0.852</v>
       </c>
       <c r="R7">
-        <v>20.3</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="S7">
-        <v>8.800000000000001</v>
+        <v>5.9</v>
       </c>
       <c r="T7">
-        <v>37.4</v>
+        <v>46</v>
       </c>
       <c r="U7">
-        <v>39.8</v>
+        <v>32.2</v>
       </c>
       <c r="V7">
-        <v>23.8</v>
+        <v>42.5</v>
       </c>
       <c r="W7" t="s">
         <v>82</v>
       </c>
       <c r="X7" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="Y7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="Z7" t="s">
         <v>71</v>
@@ -2191,94 +2221,94 @@
         <v>82</v>
       </c>
       <c r="AB7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AC7">
-        <v>166</v>
+        <v>357</v>
       </c>
       <c r="AD7">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="AE7">
-        <v>0.303</v>
+        <v>0.213</v>
       </c>
       <c r="AF7">
-        <v>0.39</v>
+        <v>0.314</v>
       </c>
       <c r="AG7">
-        <v>6.6</v>
+        <v>4.5</v>
       </c>
       <c r="AH7">
-        <v>0.243</v>
+        <v>0.21</v>
       </c>
       <c r="AI7">
-        <v>0.546</v>
+        <v>0.423</v>
       </c>
       <c r="AJ7">
-        <v>14.5</v>
+        <v>18.5</v>
       </c>
       <c r="AK7">
-        <v>7.2</v>
+        <v>10.6</v>
       </c>
       <c r="AL7">
-        <v>6.88</v>
+        <v>5.36</v>
       </c>
       <c r="AM7">
-        <v>42.5</v>
+        <v>32.7</v>
       </c>
       <c r="AN7">
-        <v>35.4</v>
+        <v>52.6</v>
       </c>
       <c r="AO7">
-        <v>24.4</v>
+        <v>12.1</v>
       </c>
       <c r="AP7">
-        <v>24.2</v>
+        <v>27.3</v>
       </c>
       <c r="AQ7">
         <v>0</v>
       </c>
       <c r="AR7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT7">
         <v>0</v>
       </c>
       <c r="AU7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW7" t="s">
         <v>64</v>
       </c>
       <c r="AX7">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="AY7">
         <v>1.5</v>
       </c>
       <c r="AZ7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB7" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="BC7" t="s">
         <v>71</v>
       </c>
       <c r="BD7" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="BE7">
-        <v>-250</v>
+        <v>-265</v>
       </c>
     </row>
     <row r="8" spans="1:57">
@@ -2295,67 +2325,67 @@
         <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>89</v>
+        <v>277</v>
       </c>
       <c r="I8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.247</v>
+        <v>0.235</v>
       </c>
       <c r="M8">
-        <v>0.353</v>
+        <v>0.309</v>
       </c>
       <c r="N8">
-        <v>0.191</v>
+        <v>0.162</v>
       </c>
       <c r="O8">
-        <v>0.362</v>
+        <v>0.306</v>
       </c>
       <c r="P8">
-        <v>0.438</v>
+        <v>0.397</v>
       </c>
       <c r="Q8">
-        <v>0.8</v>
+        <v>0.703</v>
       </c>
       <c r="R8">
-        <v>23.8</v>
+        <v>17.5</v>
       </c>
       <c r="S8">
-        <v>13.3</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="T8">
-        <v>28.1</v>
+        <v>50.9</v>
       </c>
       <c r="U8">
-        <v>53.1</v>
+        <v>29.5</v>
       </c>
       <c r="V8">
-        <v>32.8</v>
+        <v>30.8</v>
       </c>
       <c r="W8" t="s">
         <v>83</v>
       </c>
       <c r="X8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="Y8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Z8" t="s">
         <v>72</v>
@@ -2364,64 +2394,64 @@
         <v>83</v>
       </c>
       <c r="AB8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AC8">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="AD8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AE8">
-        <v>0.301</v>
+        <v>0.281</v>
       </c>
       <c r="AF8">
-        <v>0.358</v>
+        <v>0.369</v>
       </c>
       <c r="AG8">
-        <v>3.1</v>
+        <v>4.9</v>
       </c>
       <c r="AH8">
-        <v>0.176</v>
+        <v>0.222</v>
       </c>
       <c r="AI8">
-        <v>0.477</v>
+        <v>0.503</v>
       </c>
       <c r="AJ8">
-        <v>14.1</v>
+        <v>15.1</v>
       </c>
       <c r="AK8">
-        <v>6.8</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="AL8">
-        <v>4.68</v>
+        <v>5.76</v>
       </c>
       <c r="AM8">
-        <v>40.3</v>
+        <v>42.9</v>
       </c>
       <c r="AN8">
-        <v>37.6</v>
+        <v>39</v>
       </c>
       <c r="AO8">
-        <v>10.7</v>
+        <v>16.7</v>
       </c>
       <c r="AP8">
-        <v>30.5</v>
+        <v>35.7</v>
       </c>
       <c r="AQ8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR8">
         <v>1</v>
       </c>
       <c r="AS8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT8">
         <v>0</v>
       </c>
       <c r="AU8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV8">
         <v>0</v>
@@ -2430,28 +2460,28 @@
         <v>65</v>
       </c>
       <c r="AX8">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="AY8">
         <v>1.5</v>
       </c>
       <c r="AZ8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BC8" t="s">
         <v>72</v>
       </c>
       <c r="BD8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="BE8">
-        <v>-280</v>
+        <v>-265</v>
       </c>
     </row>
     <row r="9" spans="1:57">
@@ -2468,163 +2498,506 @@
         <v>66</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>94</v>
+        <v>263</v>
       </c>
       <c r="I9">
+        <v>20</v>
+      </c>
+      <c r="J9">
         <v>3</v>
       </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
       <c r="K9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>0.383</v>
+        <v>0.308</v>
       </c>
       <c r="M9">
-        <v>0.405</v>
+        <v>0.443</v>
       </c>
       <c r="N9">
-        <v>0.117</v>
+        <v>0.308</v>
       </c>
       <c r="O9">
-        <v>0.426</v>
+        <v>0.432</v>
       </c>
       <c r="P9">
-        <v>0.5</v>
+        <v>0.616</v>
       </c>
       <c r="Q9">
-        <v>0.926</v>
+        <v>1.048</v>
       </c>
       <c r="R9">
-        <v>11.8</v>
+        <v>17</v>
       </c>
       <c r="S9">
-        <v>6.9</v>
+        <v>17.9</v>
       </c>
       <c r="T9">
-        <v>41.3</v>
+        <v>43.3</v>
       </c>
       <c r="U9">
-        <v>33.8</v>
+        <v>38</v>
       </c>
       <c r="V9">
-        <v>31.3</v>
+        <v>41.9</v>
       </c>
       <c r="W9" t="s">
         <v>84</v>
       </c>
       <c r="X9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Y9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Z9" t="s">
         <v>73</v>
       </c>
       <c r="AA9" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="AB9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AC9">
-        <v>77</v>
+        <v>242</v>
       </c>
       <c r="AD9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="AE9">
-        <v>0.219</v>
+        <v>0.199</v>
       </c>
       <c r="AF9">
-        <v>0.228</v>
+        <v>0.278</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="AH9">
-        <v>0.041</v>
+        <v>0.181</v>
       </c>
       <c r="AI9">
-        <v>0.26</v>
+        <v>0.38</v>
       </c>
       <c r="AJ9">
-        <v>22.1</v>
+        <v>24.4</v>
       </c>
       <c r="AK9">
-        <v>3.9</v>
+        <v>6.2</v>
       </c>
       <c r="AL9">
-        <v>1.89</v>
+        <v>4.45</v>
       </c>
       <c r="AM9">
-        <v>69.59999999999999</v>
+        <v>29.4</v>
       </c>
       <c r="AN9">
-        <v>12.5</v>
+        <v>53.1</v>
       </c>
       <c r="AO9">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="AP9">
-        <v>26.3</v>
+        <v>28.5</v>
       </c>
       <c r="AQ9">
         <v>0</v>
       </c>
       <c r="AR9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS9">
         <v>0</v>
       </c>
       <c r="AT9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU9">
         <v>1</v>
       </c>
       <c r="AV9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW9" t="s">
         <v>66</v>
       </c>
       <c r="AX9">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="AY9">
         <v>1.5</v>
       </c>
       <c r="AZ9" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE9">
+        <v>-255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:57">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>215</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>0.326</v>
+      </c>
+      <c r="M10">
+        <v>0.382</v>
+      </c>
+      <c r="N10">
+        <v>0.172</v>
+      </c>
+      <c r="O10">
+        <v>0.383</v>
+      </c>
+      <c r="P10">
+        <v>0.498</v>
+      </c>
+      <c r="Q10">
+        <v>0.881</v>
+      </c>
+      <c r="R10">
+        <v>7.2</v>
+      </c>
+      <c r="S10">
+        <v>7.2</v>
+      </c>
+      <c r="T10">
+        <v>37.1</v>
+      </c>
+      <c r="U10">
+        <v>37.6</v>
+      </c>
+      <c r="V10">
+        <v>21.1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>85</v>
+      </c>
+      <c r="X10" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y10" t="s">
         <v>94</v>
       </c>
-      <c r="BA9" t="s">
-        <v>95</v>
-      </c>
-      <c r="BB9" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>89</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>101</v>
-      </c>
-      <c r="BE9">
-        <v>-275</v>
+      <c r="Z10" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC10">
+        <v>22</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0.095</v>
+      </c>
+      <c r="AF10">
+        <v>0.129</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0.048</v>
+      </c>
+      <c r="AI10">
+        <v>0.143</v>
+      </c>
+      <c r="AJ10">
+        <v>27.3</v>
+      </c>
+      <c r="AK10">
+        <v>4.5</v>
+      </c>
+      <c r="AL10">
+        <v>1.72</v>
+      </c>
+      <c r="AM10">
+        <v>60</v>
+      </c>
+      <c r="AN10">
+        <v>20</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>26.7</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>1</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AX10">
+        <v>180</v>
+      </c>
+      <c r="AY10">
+        <v>1.5</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>92</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>104</v>
+      </c>
+      <c r="BE10">
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:57">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>233</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>0.305</v>
+      </c>
+      <c r="M11">
+        <v>0.322</v>
+      </c>
+      <c r="N11">
+        <v>0.09</v>
+      </c>
+      <c r="O11">
+        <v>0.344</v>
+      </c>
+      <c r="P11">
+        <v>0.395</v>
+      </c>
+      <c r="Q11">
+        <v>0.739</v>
+      </c>
+      <c r="R11">
+        <v>16.5</v>
+      </c>
+      <c r="S11">
+        <v>6.3</v>
+      </c>
+      <c r="T11">
+        <v>41.7</v>
+      </c>
+      <c r="U11">
+        <v>31.3</v>
+      </c>
+      <c r="V11">
+        <v>22.3</v>
+      </c>
+      <c r="W11" t="s">
+        <v>86</v>
+      </c>
+      <c r="X11" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC11">
+        <v>229</v>
+      </c>
+      <c r="AD11">
+        <v>6</v>
+      </c>
+      <c r="AE11">
+        <v>0.214</v>
+      </c>
+      <c r="AF11">
+        <v>0.26</v>
+      </c>
+      <c r="AG11">
+        <v>2.6</v>
+      </c>
+      <c r="AH11">
+        <v>0.141</v>
+      </c>
+      <c r="AI11">
+        <v>0.355</v>
+      </c>
+      <c r="AJ11">
+        <v>22.7</v>
+      </c>
+      <c r="AK11">
+        <v>3.5</v>
+      </c>
+      <c r="AL11">
+        <v>3.16</v>
+      </c>
+      <c r="AM11">
+        <v>53</v>
+      </c>
+      <c r="AN11">
+        <v>29.2</v>
+      </c>
+      <c r="AO11">
+        <v>12.2</v>
+      </c>
+      <c r="AP11">
+        <v>26.8</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX11">
+        <v>180</v>
+      </c>
+      <c r="AY11">
+        <v>1.5</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA11" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC11" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE11">
+        <v>-250</v>
       </c>
     </row>
   </sheetData>
@@ -2634,7 +3007,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE3"/>
+  <dimension ref="A1:BE6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2815,142 +3188,142 @@
     </row>
     <row r="2" spans="1:57">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L2">
-        <v>0.364</v>
+        <v>0.333</v>
       </c>
       <c r="M2">
-        <v>0.389</v>
+        <v>0.478</v>
       </c>
       <c r="N2">
-        <v>0.182</v>
+        <v>0.378</v>
       </c>
       <c r="O2">
-        <v>0.364</v>
+        <v>0.434</v>
       </c>
       <c r="P2">
-        <v>0.545</v>
+        <v>0.711</v>
       </c>
       <c r="Q2">
-        <v>0.909</v>
+        <v>1.145</v>
       </c>
       <c r="R2">
-        <v>36.4</v>
+        <v>30.2</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="T2">
-        <v>42.9</v>
+        <v>20.7</v>
       </c>
       <c r="U2">
-        <v>14.3</v>
+        <v>41.4</v>
       </c>
       <c r="V2">
-        <v>28.6</v>
+        <v>31</v>
       </c>
       <c r="W2" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="X2" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="Y2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Z2" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="AA2" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="AB2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AC2">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="AD2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE2">
-        <v>0.301</v>
+        <v>0.522</v>
       </c>
       <c r="AF2">
-        <v>0.358</v>
+        <v>0.747</v>
       </c>
       <c r="AG2">
-        <v>3.1</v>
+        <v>20.8</v>
       </c>
       <c r="AH2">
-        <v>0.176</v>
+        <v>0.739</v>
       </c>
       <c r="AI2">
-        <v>0.477</v>
+        <v>1.261</v>
       </c>
       <c r="AJ2">
-        <v>14.1</v>
+        <v>20.8</v>
       </c>
       <c r="AK2">
-        <v>6.8</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>4.68</v>
+        <v>18.96</v>
       </c>
       <c r="AM2">
-        <v>40.3</v>
+        <v>23.5</v>
       </c>
       <c r="AN2">
-        <v>37.6</v>
+        <v>35.3</v>
       </c>
       <c r="AO2">
-        <v>10.7</v>
+        <v>83.3</v>
       </c>
       <c r="AP2">
-        <v>30.5</v>
+        <v>44.4</v>
       </c>
       <c r="AQ2">
         <v>1</v>
       </c>
       <c r="AR2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS2">
         <v>0</v>
       </c>
       <c r="AT2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU2">
         <v>1</v>
@@ -2959,165 +3332,165 @@
         <v>0</v>
       </c>
       <c r="AW2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AX2">
-        <v>-185</v>
+        <v>-155</v>
       </c>
       <c r="AY2">
         <v>0.5</v>
       </c>
       <c r="AZ2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="BA2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="BB2" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="BC2" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="BD2" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="BE2">
-        <v>135</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:57">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>54</v>
+        <v>180</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L3">
-        <v>0.315</v>
+        <v>0.333</v>
       </c>
       <c r="M3">
-        <v>0.399</v>
+        <v>0.478</v>
       </c>
       <c r="N3">
-        <v>0.259</v>
+        <v>0.378</v>
       </c>
       <c r="O3">
-        <v>0.362</v>
+        <v>0.434</v>
       </c>
       <c r="P3">
-        <v>0.574</v>
+        <v>0.711</v>
       </c>
       <c r="Q3">
-        <v>0.9360000000000001</v>
+        <v>1.145</v>
       </c>
       <c r="R3">
-        <v>27.6</v>
+        <v>30.2</v>
       </c>
       <c r="S3">
-        <v>6.9</v>
+        <v>13.2</v>
       </c>
       <c r="T3">
-        <v>35.1</v>
+        <v>20.7</v>
       </c>
       <c r="U3">
-        <v>40.5</v>
+        <v>41.4</v>
       </c>
       <c r="V3">
-        <v>28.9</v>
+        <v>31</v>
       </c>
       <c r="W3" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="X3" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="Y3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Z3" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="AA3" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="AB3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AC3">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="AD3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE3">
-        <v>0.301</v>
+        <v>0.522</v>
       </c>
       <c r="AF3">
-        <v>0.358</v>
+        <v>0.747</v>
       </c>
       <c r="AG3">
-        <v>3.1</v>
+        <v>20.8</v>
       </c>
       <c r="AH3">
-        <v>0.176</v>
+        <v>0.739</v>
       </c>
       <c r="AI3">
-        <v>0.477</v>
+        <v>1.261</v>
       </c>
       <c r="AJ3">
-        <v>14.1</v>
+        <v>20.8</v>
       </c>
       <c r="AK3">
-        <v>6.8</v>
+        <v>0</v>
       </c>
       <c r="AL3">
-        <v>4.68</v>
+        <v>18.96</v>
       </c>
       <c r="AM3">
-        <v>40.3</v>
+        <v>23.5</v>
       </c>
       <c r="AN3">
-        <v>37.6</v>
+        <v>35.3</v>
       </c>
       <c r="AO3">
-        <v>10.7</v>
+        <v>83.3</v>
       </c>
       <c r="AP3">
-        <v>30.5</v>
+        <v>44.4</v>
       </c>
       <c r="AQ3">
         <v>1</v>
       </c>
       <c r="AR3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS3">
         <v>0</v>
@@ -3132,31 +3505,550 @@
         <v>0</v>
       </c>
       <c r="AW3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="AX3">
-        <v>-245</v>
+        <v>-155</v>
       </c>
       <c r="AY3">
         <v>0.5</v>
       </c>
       <c r="AZ3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BE3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:57">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>180</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>0.333</v>
+      </c>
+      <c r="M4">
+        <v>0.478</v>
+      </c>
+      <c r="N4">
+        <v>0.378</v>
+      </c>
+      <c r="O4">
+        <v>0.434</v>
+      </c>
+      <c r="P4">
+        <v>0.711</v>
+      </c>
+      <c r="Q4">
+        <v>1.145</v>
+      </c>
+      <c r="R4">
+        <v>30.2</v>
+      </c>
+      <c r="S4">
+        <v>13.2</v>
+      </c>
+      <c r="T4">
+        <v>20.7</v>
+      </c>
+      <c r="U4">
+        <v>41.4</v>
+      </c>
+      <c r="V4">
+        <v>31</v>
+      </c>
+      <c r="W4" t="s">
+        <v>109</v>
+      </c>
+      <c r="X4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y4" t="s">
         <v>94</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="Z4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC4">
+        <v>24</v>
+      </c>
+      <c r="AD4">
+        <v>5</v>
+      </c>
+      <c r="AE4">
+        <v>0.522</v>
+      </c>
+      <c r="AF4">
+        <v>0.747</v>
+      </c>
+      <c r="AG4">
+        <v>20.8</v>
+      </c>
+      <c r="AH4">
+        <v>0.739</v>
+      </c>
+      <c r="AI4">
+        <v>1.261</v>
+      </c>
+      <c r="AJ4">
+        <v>20.8</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>18.96</v>
+      </c>
+      <c r="AM4">
+        <v>23.5</v>
+      </c>
+      <c r="AN4">
+        <v>35.3</v>
+      </c>
+      <c r="AO4">
+        <v>83.3</v>
+      </c>
+      <c r="AP4">
+        <v>44.4</v>
+      </c>
+      <c r="AQ4">
+        <v>1</v>
+      </c>
+      <c r="AR4">
+        <v>1</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>1</v>
+      </c>
+      <c r="AU4">
+        <v>1</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX4">
+        <v>-155</v>
+      </c>
+      <c r="AY4">
+        <v>0.5</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>111</v>
+      </c>
+      <c r="BE4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:57">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <v>180</v>
+      </c>
+      <c r="I5">
+        <v>16</v>
+      </c>
+      <c r="J5">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>0.333</v>
+      </c>
+      <c r="M5">
+        <v>0.478</v>
+      </c>
+      <c r="N5">
+        <v>0.378</v>
+      </c>
+      <c r="O5">
+        <v>0.434</v>
+      </c>
+      <c r="P5">
+        <v>0.711</v>
+      </c>
+      <c r="Q5">
+        <v>1.145</v>
+      </c>
+      <c r="R5">
+        <v>30.2</v>
+      </c>
+      <c r="S5">
+        <v>13.2</v>
+      </c>
+      <c r="T5">
+        <v>20.7</v>
+      </c>
+      <c r="U5">
+        <v>41.4</v>
+      </c>
+      <c r="V5">
+        <v>31</v>
+      </c>
+      <c r="W5" t="s">
+        <v>109</v>
+      </c>
+      <c r="X5" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC5">
+        <v>24</v>
+      </c>
+      <c r="AD5">
+        <v>5</v>
+      </c>
+      <c r="AE5">
+        <v>0.522</v>
+      </c>
+      <c r="AF5">
+        <v>0.747</v>
+      </c>
+      <c r="AG5">
+        <v>20.8</v>
+      </c>
+      <c r="AH5">
+        <v>0.739</v>
+      </c>
+      <c r="AI5">
+        <v>1.261</v>
+      </c>
+      <c r="AJ5">
+        <v>20.8</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>18.96</v>
+      </c>
+      <c r="AM5">
+        <v>23.5</v>
+      </c>
+      <c r="AN5">
+        <v>35.3</v>
+      </c>
+      <c r="AO5">
+        <v>83.3</v>
+      </c>
+      <c r="AP5">
+        <v>44.4</v>
+      </c>
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
+        <v>1</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX5">
+        <v>-155</v>
+      </c>
+      <c r="AY5">
+        <v>0.5</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BE5">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:57">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>128</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0.352</v>
+      </c>
+      <c r="M6">
+        <v>0.421</v>
+      </c>
+      <c r="N6">
+        <v>0.234</v>
+      </c>
+      <c r="O6">
+        <v>0.41</v>
+      </c>
+      <c r="P6">
+        <v>0.586</v>
+      </c>
+      <c r="Q6">
+        <v>0.996</v>
+      </c>
+      <c r="R6">
+        <v>20.1</v>
+      </c>
+      <c r="S6">
+        <v>7.6</v>
+      </c>
+      <c r="T6">
+        <v>38.6</v>
+      </c>
+      <c r="U6">
+        <v>41.6</v>
+      </c>
+      <c r="V6">
+        <v>45.5</v>
+      </c>
+      <c r="W6" t="s">
+        <v>110</v>
+      </c>
+      <c r="X6" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y6" t="s">
         <v>95</v>
       </c>
-      <c r="BB3" t="s">
-        <v>100</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>72</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE3">
-        <v>175</v>
+      <c r="Z6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC6">
+        <v>17</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>0.4</v>
+      </c>
+      <c r="AF6">
+        <v>0.506</v>
+      </c>
+      <c r="AG6">
+        <v>5.9</v>
+      </c>
+      <c r="AH6">
+        <v>0.333</v>
+      </c>
+      <c r="AI6">
+        <v>0.733</v>
+      </c>
+      <c r="AJ6">
+        <v>5.9</v>
+      </c>
+      <c r="AK6">
+        <v>11.8</v>
+      </c>
+      <c r="AL6">
+        <v>8.24</v>
+      </c>
+      <c r="AM6">
+        <v>21.4</v>
+      </c>
+      <c r="AN6">
+        <v>42.9</v>
+      </c>
+      <c r="AO6">
+        <v>16.7</v>
+      </c>
+      <c r="AP6">
+        <v>35.7</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>1</v>
+      </c>
+      <c r="AU6">
+        <v>1</v>
+      </c>
+      <c r="AV6">
+        <v>1</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>106</v>
+      </c>
+      <c r="AX6">
+        <v>-260</v>
+      </c>
+      <c r="AY6">
+        <v>0.5</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>98</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>108</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>112</v>
+      </c>
+      <c r="BE6">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>